<commit_message>
Task 6 done and updated for 4/5 revisions
</commit_message>
<xml_diff>
--- a/raw_data/CPA_ProjectReportTemplate_IntroductionToMarketing_2023_Fall_20231031p.xlsx
+++ b/raw_data/CPA_ProjectReportTemplate_IntroductionToMarketing_2023_Fall_20231031p.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="group"/>
@@ -1898,7 +1898,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1958,8 +1958,12 @@
       <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="5">
@@ -2121,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>10.329</v>
+        <v>5.83898</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
@@ -2129,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>10.20939</v>
+        <v>3.26256</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
@@ -2137,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>10.09118</v>
+        <v>1.82297</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
@@ -2145,7 +2149,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="7">
-        <v>9.97433</v>
+        <v>1.01859</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
@@ -2153,7 +2157,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>9.85883</v>
+        <v>0.56914</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
@@ -2161,7 +2165,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="7">
-        <v>9.74468</v>
+        <v>0.31801</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
@@ -2169,7 +2173,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <v>9.63184</v>
+        <v>0.17769</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
@@ -2177,7 +2181,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="7">
-        <v>9.52031</v>
+        <v>0.09929</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
@@ -2185,7 +2189,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="7">
-        <v>9.41007</v>
+        <v>0.05548</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
@@ -2193,7 +2197,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="7">
-        <v>9.30111</v>
+        <v>0.031</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
@@ -2201,7 +2205,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="7">
-        <v>9.19341</v>
+        <v>0.01732</v>
       </c>
     </row>
   </sheetData>
@@ -2216,7 +2220,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2236,7 +2240,9 @@
       <c r="A2" s="7">
         <v>12.69215</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="7">
+        <v>23.756171562770646</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>